<commit_message>
Tested ordering and cart
</commit_message>
<xml_diff>
--- a/CommonBase/data.xlsx
+++ b/CommonBase/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://persistentsystems-my.sharepoint.com/personal/shane_furtado_persistent_com1/Documents/Documents/Automation/SauceDemoTesting/CommonBase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{DB79B778-225B-4401-9E76-3A1B23EEC646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2349CD68-A14C-4A2C-AEFF-9B8631464E79}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="13_ncr:1_{DB79B778-225B-4401-9E76-3A1B23EEC646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C454E57-BF96-4605-A0F0-92066D29764F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{FAB23016-B0A3-4F77-A62F-EB6DCA33B0C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{FAB23016-B0A3-4F77-A62F-EB6DCA33B0C6}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="fields" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>standard_user</t>
   </si>
@@ -66,6 +67,45 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>dfdfre</t>
+  </si>
+  <si>
+    <t>e34re2</t>
+  </si>
+  <si>
+    <t>aaaaaa</t>
+  </si>
+  <si>
+    <t>fdfsfbf</t>
+  </si>
+  <si>
+    <t>ererer</t>
+  </si>
+  <si>
+    <t>rrgds</t>
+  </si>
+  <si>
+    <t>sdvsbsfb</t>
+  </si>
+  <si>
+    <t>qddddd</t>
+  </si>
+  <si>
+    <t>shane</t>
+  </si>
+  <si>
+    <t>fgvdse332</t>
   </si>
 </sst>
 </file>
@@ -118,6 +158,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0A767D-4323-428D-B090-FADDC8D55698}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -504,6 +548,116 @@
       </c>
       <c r="C7" t="s">
         <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAFAACE0-505D-4C9F-A2CF-98D55E306CE4}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>463723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>333453</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>342113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>343434</v>
+      </c>
+      <c r="D4">
+        <v>403601</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>313</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>33333</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -745,20 +899,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d256ee5c-265a-405e-bc7a-ae550e4568c2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d256ee5c-265a-405e-bc7a-ae550e4568c2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,14 +935,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E715FCB3-A71F-4088-BF3D-5481A6E28B06}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F56B8D9-3190-4452-B5BD-E69BC46C6857}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -805,6 +951,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E715FCB3-A71F-4088-BF3D-5481A6E28B06}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{1f4beacd-b7aa-49b2-aaa1-b8525cb257e0}" enabled="0" method="" siteId="{1f4beacd-b7aa-49b2-aaa1-b8525cb257e0}" removed="1"/>

</xml_diff>